<commit_message>
Apr-27-driver script for app login
</commit_message>
<xml_diff>
--- a/FileInput/DataEngine.xlsx
+++ b/FileInput/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Liveproject\ERP_hybrid_StockAccounting\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1DEDFA-4AA7-411C-B3DE-91C1F8A0D700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09C5B2-C803-4E34-8046-DB3535EEA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{295DEF63-B58F-40DC-859C-6D26F030B969}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>TCID</t>
   </si>
@@ -173,9 +173,6 @@
     <t>validateTitle</t>
   </si>
   <si>
-    <t xml:space="preserve">Dashboard « Stock Accounting </t>
-  </si>
-  <si>
     <t>Click Logout button</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>launchUrl</t>
+  </si>
+  <si>
+    <t>Dashboard « Stock Accounting</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +780,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
@@ -878,8 +878,8 @@
       <c r="D8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>22</v>
+      <c r="E8" s="10">
+        <v>10</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -897,13 +897,13 @@
         <v>22</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>36</v>
@@ -921,11 +921,11 @@
     </row>
     <row r="11" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
@@ -938,52 +938,52 @@
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>

</xml_diff>

<commit_message>
Supplier functions and script to run testcase present in excel through keywords
</commit_message>
<xml_diff>
--- a/FileInput/DataEngine.xlsx
+++ b/FileInput/DataEngine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Liveproject\ERP_hybrid_StockAccounting\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09C5B2-C803-4E34-8046-DB3535EEA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD11293-3EB6-4EB6-B168-1897BB75FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{295DEF63-B58F-40DC-859C-6D26F030B969}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{295DEF63-B58F-40DC-859C-6D26F030B969}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -186,6 +186,204 @@
   </si>
   <si>
     <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>//a[starts-with(text(),'Stock Items ')]</t>
+  </si>
+  <si>
+    <t>wait for stockitems</t>
+  </si>
+  <si>
+    <t>Click add button</t>
+  </si>
+  <si>
+    <t>Wait for category name</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Category_Name']</t>
+  </si>
+  <si>
+    <t>Enter category name</t>
+  </si>
+  <si>
+    <t>purifier by sasi</t>
+  </si>
+  <si>
+    <t>Click on Add button</t>
+  </si>
+  <si>
+    <t>//button[@id='btnAction']</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>Wait for confirm ok button</t>
+  </si>
+  <si>
+    <t>wait for alert ok button</t>
+  </si>
+  <si>
+    <t>//div[@class='ajs-header']</t>
+  </si>
+  <si>
+    <t>Click on ok button</t>
+  </si>
+  <si>
+    <t>//button[@class='ajs-button btn btn-primary']</t>
+  </si>
+  <si>
+    <t>Validate category table</t>
+  </si>
+  <si>
+    <t>Close App browser</t>
+  </si>
+  <si>
+    <t>mouseClick</t>
+  </si>
+  <si>
+    <t>Mouse click to stock items</t>
+  </si>
+  <si>
+    <t>categoryTable</t>
+  </si>
+  <si>
+    <t>(//a[@data-original-title='Add'])[1]</t>
+  </si>
+  <si>
+    <t>wait for add button</t>
+  </si>
+  <si>
+    <t>Wait for suppliers link</t>
+  </si>
+  <si>
+    <t>(//a[contains(text(),'Suppliers')])[2]</t>
+  </si>
+  <si>
+    <t>Click on suppliers link</t>
+  </si>
+  <si>
+    <t>Wait for Add button</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Add button </t>
+  </si>
+  <si>
+    <t>wait for supplier number</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Supplier_Number']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Supplier name </t>
+  </si>
+  <si>
+    <t>//input[@id='x_Supplier_Name']</t>
+  </si>
+  <si>
+    <t>Capture supplier number</t>
+  </si>
+  <si>
+    <t>Enter Address</t>
+  </si>
+  <si>
+    <t>Enter city</t>
+  </si>
+  <si>
+    <t>Enter country</t>
+  </si>
+  <si>
+    <t>Enter contact person</t>
+  </si>
+  <si>
+    <t>Enter Phone number</t>
+  </si>
+  <si>
+    <t>Enter Email</t>
+  </si>
+  <si>
+    <t>Enter mobilenumber</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Click Add button</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Address']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_City']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Country']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Contact_Person']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Phone_Number']</t>
+  </si>
+  <si>
+    <t>//input[@id='x__Email']</t>
+  </si>
+  <si>
+    <t>//input[@id='x_Mobile_Number']</t>
+  </si>
+  <si>
+    <t>//textarea[@id='x_Notes']</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>sasi</t>
+  </si>
+  <si>
+    <t>bangalore</t>
+  </si>
+  <si>
+    <t>india</t>
+  </si>
+  <si>
+    <t>gmail.com</t>
+  </si>
+  <si>
+    <t>some notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait for confirm ok button </t>
+  </si>
+  <si>
+    <t>click on confirm add button</t>
+  </si>
+  <si>
+    <t>(//button[contains(.,'OK')])[6]</t>
+  </si>
+  <si>
+    <t>click on alert ok button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate supplier table </t>
+  </si>
+  <si>
+    <t>supplierTable</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Close app browser</t>
+  </si>
+  <si>
+    <t>CaptureSnumber</t>
+  </si>
+  <si>
+    <t>Supplier-00000000075</t>
   </si>
 </sst>
 </file>
@@ -294,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -312,6 +510,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +828,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -674,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -724,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8DAF5F-DCFB-452C-B25A-AE1E48A9D87E}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,25 +1200,974 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511E9A88-8880-47E8-AF09-0489ADD51FD0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="10">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="10">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="10">
+        <v>10</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EA7F61-7C1E-4428-8269-7F1D47464321}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="10">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="10">
+        <v>4327575</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="10">
+        <v>4365475</v>
+      </c>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="10">
+        <v>10</v>
+      </c>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="10">
+        <v>10</v>
+      </c>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excel forgot to stage
</commit_message>
<xml_diff>
--- a/FileInput/DataEngine.xlsx
+++ b/FileInput/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Liveproject\ERP_hybrid_StockAccounting\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD11293-3EB6-4EB6-B168-1897BB75FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13F0C0E-64D5-4269-8915-689F7B2E00E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{295DEF63-B58F-40DC-859C-6D26F030B969}"/>
   </bookViews>
@@ -1589,7 +1589,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1833,7 +1833,7 @@
         <v>78</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="F13" s="10"/>
     </row>

</xml_diff>